<commit_message>
Energy vs. size graph.
</commit_message>
<xml_diff>
--- a/chapters/ch07-Households/datasets/ce2.1.xlsx
+++ b/chapters/ch07-Households/datasets/ce2.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch07-Households/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FE53F3-7342-CD46-9041-E096B1216C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45831D32-B22F-014D-9FB2-74E0388D4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="460" windowWidth="22180" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1074,15 +1074,6 @@
     <t>&lt; 1000</t>
   </si>
   <si>
-    <t>1000–1499</t>
-  </si>
-  <si>
-    <t>1500–1999</t>
-  </si>
-  <si>
-    <t>2000–2499</t>
-  </si>
-  <si>
     <t>2500-2999</t>
   </si>
   <si>
@@ -1099,6 +1090,15 @@
   </si>
   <si>
     <t>&gt; 3000</t>
+  </si>
+  <si>
+    <t>1000-1499</t>
+  </si>
+  <si>
+    <t>1500-1999</t>
+  </si>
+  <si>
+    <t>2000-2499</t>
   </si>
 </sst>
 </file>
@@ -1776,7 +1776,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1786,16 +1786,16 @@
         <v>114</v>
       </c>
       <c r="B1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1">
         <f>Btu!I63</f>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B4" s="1">
         <f>Btu!I64</f>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1">
         <f>Btu!I65</f>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1">
         <f>Btu!I66</f>
@@ -1906,7 +1906,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B7" s="1">
         <f>Btu!I67</f>

</xml_diff>

<commit_message>
New calcs for housing energy use.
</commit_message>
<xml_diff>
--- a/chapters/ch07-Households/datasets/ce2.1.xlsx
+++ b/chapters/ch07-Households/datasets/ce2.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch07-Households/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45831D32-B22F-014D-9FB2-74E0388D4D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19670C09-D988-C742-BE11-3817D330B874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="460" windowWidth="22180" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20340" yWindow="460" windowWidth="28020" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="9" r:id="rId1"/>
@@ -28,9 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="126">
   <si>
     <t>Number of housing units (million)</t>
   </si>
@@ -1775,7 +1773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C06240-1322-4646-837C-BB33A572CEE3}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1935,11 +1933,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T62" sqref="T62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3701,7 +3699,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>36</v>
       </c>
@@ -3739,7 +3737,7 @@
         <v>82.2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>105</v>
       </c>
@@ -3777,7 +3775,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>33</v>
       </c>
@@ -3815,7 +3813,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>24</v>
       </c>
@@ -3853,7 +3851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>25</v>
       </c>
@@ -3891,7 +3889,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>26</v>
       </c>
@@ -3929,7 +3927,7 @@
         <v>79.900000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>27</v>
       </c>
@@ -3967,7 +3965,7 @@
         <v>63.2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>28</v>
       </c>
@@ -4005,7 +4003,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>29</v>
       </c>
@@ -4043,7 +4041,7 @@
         <v>58.6</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>30</v>
       </c>
@@ -4081,7 +4079,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>31</v>
       </c>
@@ -4119,7 +4117,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>32</v>
       </c>
@@ -4157,7 +4155,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>107</v>
       </c>
@@ -4194,8 +4192,20 @@
       <c r="L61" s="22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O61" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="P61" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q61" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="R61" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>37</v>
       </c>
@@ -4232,8 +4242,28 @@
       <c r="L62" s="23">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O62" s="1">
+        <f>D62/$B62</f>
+        <v>22.593984962406015</v>
+      </c>
+      <c r="P62" s="1">
+        <f t="shared" ref="P62:R62" si="0">E62/$B62</f>
+        <v>15.263157894736841</v>
+      </c>
+      <c r="Q62" s="1">
+        <f t="shared" si="0"/>
+        <v>0.93984962406015038</v>
+      </c>
+      <c r="R62" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4661654135338344</v>
+      </c>
+      <c r="T62" s="1">
+        <f>SUM(O62:R62)</f>
+        <v>40.263157894736842</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>38</v>
       </c>
@@ -4270,8 +4300,28 @@
       <c r="L63" s="23">
         <v>41</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O63" s="1">
+        <f t="shared" ref="O63:O67" si="1">D63/$B63</f>
+        <v>34.214559386973178</v>
+      </c>
+      <c r="P63" s="1">
+        <f t="shared" ref="P63:P67" si="2">E63/$B63</f>
+        <v>22.030651340996169</v>
+      </c>
+      <c r="Q63" s="1">
+        <f t="shared" ref="Q63:Q67" si="3">F63/$B63</f>
+        <v>1.4942528735632183</v>
+      </c>
+      <c r="R63" s="1">
+        <f t="shared" ref="R63:R67" si="4">G63/$B63</f>
+        <v>1.3409961685823755</v>
+      </c>
+      <c r="T63" s="1">
+        <f t="shared" ref="T63:T67" si="5">SUM(O63:R63)</f>
+        <v>59.080459770114949</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>39</v>
       </c>
@@ -4308,8 +4358,28 @@
       <c r="L64" s="23">
         <v>60.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O64" s="1">
+        <f t="shared" si="1"/>
+        <v>39.942857142857143</v>
+      </c>
+      <c r="P64" s="1">
+        <f t="shared" si="2"/>
+        <v>31.885714285714286</v>
+      </c>
+      <c r="Q64" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5714285714285716</v>
+      </c>
+      <c r="R64" s="1">
+        <f t="shared" si="4"/>
+        <v>3.2571428571428571</v>
+      </c>
+      <c r="T64" s="1">
+        <f t="shared" si="5"/>
+        <v>77.657142857142844</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>40</v>
       </c>
@@ -4346,8 +4416,28 @@
       <c r="L65" s="23">
         <v>68.099999999999994</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O65" s="1">
+        <f t="shared" si="1"/>
+        <v>39.645390070921984</v>
+      </c>
+      <c r="P65" s="1">
+        <f t="shared" si="2"/>
+        <v>41.418439716312058</v>
+      </c>
+      <c r="Q65" s="1">
+        <f t="shared" si="3"/>
+        <v>4.9645390070921991</v>
+      </c>
+      <c r="R65" s="1">
+        <f t="shared" si="4"/>
+        <v>3.9007092198581561</v>
+      </c>
+      <c r="T65" s="1">
+        <f t="shared" si="5"/>
+        <v>89.929078014184398</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>42</v>
       </c>
@@ -4384,8 +4474,28 @@
       <c r="L66" s="23">
         <v>85.1</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O66" s="1">
+        <f t="shared" si="1"/>
+        <v>41.851851851851848</v>
+      </c>
+      <c r="P66" s="1">
+        <f t="shared" si="2"/>
+        <v>49.722222222222221</v>
+      </c>
+      <c r="Q66" s="1">
+        <f t="shared" si="3"/>
+        <v>3.4259259259259256</v>
+      </c>
+      <c r="R66" s="1">
+        <f t="shared" si="4"/>
+        <v>7.8703703703703702</v>
+      </c>
+      <c r="T66" s="1">
+        <f t="shared" si="5"/>
+        <v>102.87037037037037</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>41</v>
       </c>
@@ -4422,8 +4532,28 @@
       <c r="L67" s="23">
         <v>91.3</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O67" s="1">
+        <f t="shared" si="1"/>
+        <v>48.484848484848484</v>
+      </c>
+      <c r="P67" s="1">
+        <f t="shared" si="2"/>
+        <v>56.493506493506487</v>
+      </c>
+      <c r="Q67" s="1">
+        <f t="shared" si="3"/>
+        <v>6.2770562770562766</v>
+      </c>
+      <c r="R67" s="1">
+        <f t="shared" si="4"/>
+        <v>8.3116883116883109</v>
+      </c>
+      <c r="T67" s="1">
+        <f t="shared" si="5"/>
+        <v>119.56709956709956</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>43</v>
       </c>
@@ -4461,7 +4591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>44</v>
       </c>
@@ -4499,7 +4629,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>45</v>
       </c>
@@ -4537,7 +4667,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
         <v>46</v>
       </c>
@@ -4575,7 +4705,7 @@
         <v>75.599999999999994</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>47</v>
       </c>
@@ -4613,7 +4743,7 @@
         <v>75.7</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>48</v>
       </c>
@@ -4651,7 +4781,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>49</v>
       </c>
@@ -4689,7 +4819,7 @@
         <v>99.3</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>50</v>
       </c>
@@ -4727,7 +4857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>51</v>
       </c>
@@ -4765,7 +4895,7 @@
         <v>53.9</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>52</v>
       </c>
@@ -4803,7 +4933,7 @@
         <v>64.8</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>53</v>
       </c>
@@ -4841,7 +4971,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>54</v>
       </c>
@@ -4879,7 +5009,7 @@
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Fixing units on avg home energy consumption. #117
</commit_message>
<xml_diff>
--- a/chapters/ch07-Households/datasets/ce2.1.xlsx
+++ b/chapters/ch07-Households/datasets/ce2.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch07-Households/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19670C09-D988-C742-BE11-3817D330B874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DAA987-014F-D949-9C05-40E4DBA6DAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20340" yWindow="460" windowWidth="28020" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -1773,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C06240-1322-4646-837C-BB33A572CEE3}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1802,20 +1804,20 @@
         <v>116</v>
       </c>
       <c r="B2">
-        <f>Btu!I62</f>
-        <v>22.6</v>
+        <f>Btu!O62</f>
+        <v>22.593984962406015</v>
       </c>
       <c r="C2" s="1">
-        <f>Btu!J62</f>
-        <v>27.5</v>
+        <f>Btu!P62</f>
+        <v>15.263157894736841</v>
       </c>
       <c r="D2" s="1">
-        <f>Btu!K62</f>
-        <v>16.5</v>
+        <f>Btu!Q62</f>
+        <v>0.93984962406015038</v>
       </c>
       <c r="E2" s="1">
-        <f>Btu!L62</f>
-        <v>33.299999999999997</v>
+        <f>Btu!R62</f>
+        <v>1.4661654135338344</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1823,20 +1825,20 @@
         <v>123</v>
       </c>
       <c r="B3" s="1">
-        <f>Btu!I63</f>
-        <v>34.200000000000003</v>
+        <f>Btu!O63</f>
+        <v>34.214559386973178</v>
       </c>
       <c r="C3" s="1">
-        <f>Btu!J63</f>
-        <v>44.4</v>
+        <f>Btu!P63</f>
+        <v>22.030651340996169</v>
       </c>
       <c r="D3" s="1">
-        <f>Btu!K63</f>
-        <v>20</v>
+        <f>Btu!Q63</f>
+        <v>1.4942528735632183</v>
       </c>
       <c r="E3" s="1">
-        <f>Btu!L63</f>
-        <v>41</v>
+        <f>Btu!R63</f>
+        <v>1.3409961685823755</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1844,20 +1846,20 @@
         <v>124</v>
       </c>
       <c r="B4" s="1">
-        <f>Btu!I64</f>
-        <v>40</v>
+        <f>Btu!O64</f>
+        <v>39.942857142857143</v>
       </c>
       <c r="C4" s="1">
-        <f>Btu!J64</f>
-        <v>56.3</v>
+        <f>Btu!P64</f>
+        <v>31.885714285714286</v>
       </c>
       <c r="D4" s="1">
-        <f>Btu!K64</f>
-        <v>25.8</v>
+        <f>Btu!Q64</f>
+        <v>2.5714285714285716</v>
       </c>
       <c r="E4" s="1">
-        <f>Btu!L64</f>
-        <v>60.4</v>
+        <f>Btu!R64</f>
+        <v>3.2571428571428571</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1865,20 +1867,20 @@
         <v>125</v>
       </c>
       <c r="B5" s="1">
-        <f>Btu!I65</f>
-        <v>39.6</v>
+        <f>Btu!O65</f>
+        <v>39.645390070921984</v>
       </c>
       <c r="C5" s="1">
-        <f>Btu!J65</f>
-        <v>68.3</v>
+        <f>Btu!P65</f>
+        <v>41.418439716312058</v>
       </c>
       <c r="D5" s="1">
-        <f>Btu!K65</f>
-        <v>38.9</v>
+        <f>Btu!Q65</f>
+        <v>4.9645390070921991</v>
       </c>
       <c r="E5" s="1">
-        <f>Btu!L65</f>
-        <v>68.099999999999994</v>
+        <f>Btu!R65</f>
+        <v>3.9007092198581561</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1886,20 +1888,20 @@
         <v>117</v>
       </c>
       <c r="B6" s="1">
-        <f>Btu!I66</f>
-        <v>41.9</v>
+        <f>Btu!O66</f>
+        <v>41.851851851851848</v>
       </c>
       <c r="C6" s="1">
-        <f>Btu!J66</f>
-        <v>74.900000000000006</v>
+        <f>Btu!P66</f>
+        <v>49.722222222222221</v>
       </c>
       <c r="D6" s="1">
-        <f>Btu!K66</f>
-        <v>30.3</v>
+        <f>Btu!Q66</f>
+        <v>3.4259259259259256</v>
       </c>
       <c r="E6" s="1">
-        <f>Btu!L66</f>
-        <v>85.1</v>
+        <f>Btu!R66</f>
+        <v>7.8703703703703702</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1907,20 +1909,20 @@
         <v>122</v>
       </c>
       <c r="B7" s="1">
-        <f>Btu!I67</f>
-        <v>48.5</v>
+        <f>Btu!O67</f>
+        <v>48.484848484848484</v>
       </c>
       <c r="C7" s="1">
-        <f>Btu!J67</f>
-        <v>85.3</v>
+        <f>Btu!P67</f>
+        <v>56.493506493506487</v>
       </c>
       <c r="D7" s="1">
-        <f>Btu!K67</f>
-        <v>43.3</v>
+        <f>Btu!Q67</f>
+        <v>6.2770562770562766</v>
       </c>
       <c r="E7" s="1">
-        <f>Btu!L67</f>
-        <v>91.3</v>
+        <f>Btu!R67</f>
+        <v>8.3116883116883109</v>
       </c>
     </row>
   </sheetData>
@@ -1935,7 +1937,7 @@
   </sheetPr>
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T62" sqref="T62"/>
     </sheetView>

</xml_diff>